<commit_message>
update documentation of the repo
</commit_message>
<xml_diff>
--- a/docs/angular.xlsx
+++ b/docs/angular.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\ng-brillio-2019-06-17\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF28F98C-B2B3-4CE2-A944-D8FFCCAC461D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73F7E2D-5E15-4E92-80E9-A9659F4A2FC2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{127AE8B2-EE5E-4B48-A629-74B7F2081CC4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>GitHub Repo:</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Contains the system requirements for the workshop. Participants are supposed to setup the pre-requisite software tools on their laptops in order to work with demo apps and projects</t>
   </si>
   <si>
-    <t>Contains slides for Redux. Covered on day 3</t>
-  </si>
-  <si>
     <t>'apps' Folder</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>Contains slides for Angular Modules (ngModule)</t>
   </si>
   <si>
-    <t>Contains slides for unit testing Angular apps</t>
-  </si>
-  <si>
     <t>A document for RxJS Observable</t>
   </si>
   <si>
@@ -187,6 +181,158 @@
   </si>
   <si>
     <t>misc-files</t>
+  </si>
+  <si>
+    <t>This app is the first and basic Angular app of the course. This is created to understand:
+1. How to create and run an Angular app using Angular CLI (https://angular.io/cli)
+2. Angular project structure (https://angular.io/guide/file-structure)
+3. Bootstrapping process (https://angular.io/guide/bootstrapping)</t>
+  </si>
+  <si>
+    <t>Contains code examples for various concepts in TypeScript. Files have been named appropriately after the concept names. For e.g., 'template-strings.ts' contains demo code for template literal (also called template sting) of TypeScript / ES6</t>
+  </si>
+  <si>
+    <t>This app can be used as a reference by participants. It contains the code to demonstrate the usage of all lifecycle hooks.</t>
+  </si>
+  <si>
+    <t>This app is used to understand and apply various Component Lifecyle Hooks (https://angular.io/guide/lifecycle-hooks). The start project provides a foundation to the participants to implement component lifecycle methods. It provides a hands-on experience to the participants who would like to code along with the instructor</t>
+  </si>
+  <si>
+    <t>We continue with the day 2 'store-app' and understand &amp; apply the following concepts:
+1. The need for creating small components
+2. How to refactor bigger components into smaller, more focussed components that follow 'Single Responsibility Principle'
+3. How do components interact with each other? (https://angular.io/guide/component-interaction)
+    a. Parent to child interaction
+    b. Child to parent interaction</t>
+  </si>
+  <si>
+    <t>We make a new copy the above app. This app will be used to understand:
+1. What is a Service? What is the need for a service?
+2. What is Dependency Injection (DI)? Why DI? What are the techniques to implement DI? 
+    (https://angular.io/guide/dependency-injection)
+3. How to consume a service in a component?
+4. What is a provider?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We continue with day 3 'store-app-services' app to learn more about services:
+1. Understanding provider scope
+2. How a service can be used in component interaction?
+We also learn:
+1. How to create a custom directive?
+2. How to create a custom pipe? </t>
+  </si>
+  <si>
+    <t>This app contains completed demo code for handling forms, both Template-driven and Reactive approaches. Participants can use this app as a reference</t>
+  </si>
+  <si>
+    <t>This app contains completed demo code for routing and navigation. Participants can use this app as a reference</t>
+  </si>
+  <si>
+    <t>Contains important links to various Angular articles and YouTube videos. Participants can use these links as reference</t>
+  </si>
+  <si>
+    <t>This folder contains code samples for using RxJS Observables and various operators. The participant will learn:
+1. What is an Observable? Why Observable? (https://angular.io/guide/observables)
+2. Different techniques to create observables
+3. Apply numerous operators on observables</t>
+  </si>
+  <si>
+    <t>This app is used to learn and apply routing and navigation within Angular apps. The Angular Router enables navigation from one view to another view (https://angular.io/guide/router). It helps the participant to:
+1. Define application routes and register them with the Router module
+2. Understand and use various routing related directives like &lt;router-outlet&gt;, routerLink, routerLinkActive, etc.
+3. Define wildcard route
+4. Define and retrieve route parameters
+5. Configure child routes
+6. Passing query parameters
+7. Understand the concept of route guards
+8. How to navigate programmatically using Router service?
+The start project can be used by the participants to get hands-on coding experience along with the instructor.</t>
+  </si>
+  <si>
+    <t>This app contains completed demo code for HTTP communcation with the server API. Participants can use this app as a reference</t>
+  </si>
+  <si>
+    <t>1. Contains server-api.json
+2. This file is used to simulate server-side REST API that is needed for the application
+3. 'json-server' tool is used to simulate a server. See '1-angular-workshop-lab-setup.pdf' document (docs folder) to know more about json-server</t>
+  </si>
+  <si>
+    <t>1. Contains server-api.json
+2. This file is used to simulate server-side REST API that is needed for the unit testing app
+3. 'json-server' tool is used to simulate a server. See '1-angular-workshop-lab-setup.pdf' document (docs folder) to know more about json-server</t>
+  </si>
+  <si>
+    <t>This app contains code for demonstrating various unit and integration test scenarios within an Angular app. (https://angular.io/guide/testing). The participant will learn about:
+1. Fundamentals of Angular testing
+2. Setup and Tear Down
+3. What are Spies? Why Spies?
+4. Code Coverage
+5. Angular Testing Utilities
+6. Testing Components
+7. Handling Component Dependencies
+8. Testing Async Operations</t>
+  </si>
+  <si>
+    <t>Contains slides for Angular Unit Testing</t>
+  </si>
+  <si>
+    <t>Contains code examples for following concepts in TypeScript / ES6:
+1. Object literal short-hand notation in ES6
+2. Destructuring - Array and Object
+3. Modules, Import, Export</t>
+  </si>
+  <si>
+    <t>This app is created to understand:
+1. The organization of an Angular application
+2. How to install Bootstrap and how to include a reference to it within the app
+3. What is an Angular Module (ngModule)?
+4. What is a Component? What does a Component consist of?
+5. What is a Decorator? What is its purpose? Understand @NgModule and @Component decorators
+6. What is a root module? What is a root component?
+7. How to create components? How to compose simple components and create complex components
+8. What are component templates and styles? How to specify inline and external templates and styles for a component
+8. What are the various data binding techniques? How to use them?
+9. What is a Directive? What are the types? Examples of using built-in directives like ngModel, ngClass, ngStyle, ngFor, ngIf, etc.
+10. What is a Pipe? Examples of using built-in pipes like date, uppercase, currency. How to chain pipes?
+At the end of day 1, participants will have a small, running Product Store application on their laptops.</t>
+  </si>
+  <si>
+    <t>This app is used to learn different types of form handling in Angular. It helps the participants to understand:
+1. Different approaches to handle user input through forms (https://angular.io/guide/forms-overview)
+    a. Template driven forms (https://angular.io/guide/forms)
+    b. Reactive forms (https://angular.io/guide/reactive-forms)
+2. The usage of various built-in validators
+3. How to create and use custom validators?
+4. How to create and use async validators?
+5. Various states of form and form controls
+6. How to set or retrieve values from form controls?
+7. Various directives used for template driven and reactive forms
+The start project can be used by the participants to get hands-on coding experience along with the instructor.</t>
+  </si>
+  <si>
+    <t>This folder contains code samples for asynchronous JavaScript. The participant will learn different techniques to write async code in JavaScript:
+1. Using callbacks
+2. Using promises</t>
+  </si>
+  <si>
+    <t>This app helps the participant to learn about server communication (HTTP) from Angular applications. This app helps participant to understand:
+1. How to communicate with the server via HTTP protocol using HttpClient service? (https://angular.io/guide/http)
+2. Getting JSON data from a server-side REST API
+3. Sending data to the server
+    a. Making a POST request
+    b. Making a DELETE request
+    c. Making a PUT/PATCH request
+    d. Adding headers
+4. Adding URL parameters
+5. How to handle errors?
+6. Understand the concept of interceptors
+The start project can be used by the participants to get hands-on coding experience along with the instructor.</t>
+  </si>
+  <si>
+    <t>Contains HTML markup for:
+1. Product Detail Component
+2. Product Form Component
+Also, it contains Products JSON file used for simulating server side REST API</t>
   </si>
 </sst>
 </file>
@@ -351,6 +497,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -362,16 +518,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -691,7 +837,7 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,17 +847,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="8"/>
+      <c r="A1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="12"/>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>15</v>
+      <c r="B3" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -723,7 +869,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -731,15 +877,15 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -751,10 +897,10 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="10"/>
+      <c r="B12" s="14"/>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
@@ -766,7 +912,7 @@
     </row>
     <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>10</v>
@@ -774,61 +920,61 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="10"/>
+      <c r="B22" s="14"/>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>9</v>
@@ -836,191 +982,233 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="3"/>
+    <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
-      <c r="B27" s="14"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="3"/>
+    <row r="29" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="14"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="10"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="3"/>
+    <row r="33" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="3"/>
+      <c r="B36" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="10"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="9"/>
+      <c r="B44" s="10"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A51" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="9"/>
+      <c r="B53" s="10"/>
+    </row>
+    <row r="54" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="13"/>
-      <c r="B42" s="14"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" s="3"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B48" s="3"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" s="3"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="13"/>
-      <c r="B53" s="14"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B54" s="3"/>
+      <c r="B54" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A6:A8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A6:A8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{4F979A98-58D0-4F26-9BBD-FE4FCAB52A97}"/>

</xml_diff>